<commit_message>
them thu muc huong dan nop bai
</commit_message>
<xml_diff>
--- a/Để nộp/danh_sach_nhom.xlsx
+++ b/Để nộp/danh_sach_nhom.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\UIT\4th Semester\[CS106] Artifical Intelligence\LAB\LAB01\BaiTap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\UIT\UIT\4th Semester\[CS106] Artifical Intelligence\LAB\LAB02\Để nộp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9DB4B3-0131-4F51-9219-E76B74CE0647}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6EC3658-90B8-4CB7-884B-6CFEFA191AF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -52,13 +52,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF444950"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -81,11 +87,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,10 +373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C10" sqref="C10:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,13 +412,26 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
+      <c r="B3">
+        <v>18521654</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
+      <c r="B4" s="1">
+        <v>18521297</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>